<commit_message>
CS107-7: Added getNameById method to driver with test and updated studentData with meaningful names
</commit_message>
<xml_diff>
--- a/plagiarism-detector/src/test/resources/studentData.xlsx
+++ b/plagiarism-detector/src/test/resources/studentData.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41A4328-7672-479B-8D65-850AF83BA373}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{B4C51E10-F811-4730-9402-B0D82D5FAC73}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10700" windowHeight="3440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,21 +38,9 @@
     <t>s.s@husky.neu.edu</t>
   </si>
   <si>
-    <t>shail</t>
-  </si>
-  <si>
     <t>s.sh@husky.neu.edu</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
@@ -68,6 +57,18 @@
   </si>
   <si>
     <t>i</t>
+  </si>
+  <si>
+    <t>Darshan</t>
+  </si>
+  <si>
+    <t>Shail</t>
+  </si>
+  <si>
+    <t>Vaibhav</t>
+  </si>
+  <si>
+    <t>John</t>
   </si>
 </sst>
 </file>
@@ -399,7 +400,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -425,7 +426,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -436,10 +437,10 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -447,10 +448,10 @@
         <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -458,10 +459,10 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -469,10 +470,10 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -480,10 +481,10 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -491,10 +492,10 @@
         <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -502,10 +503,10 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -513,10 +514,10 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -524,10 +525,10 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -535,10 +536,10 @@
         <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CS107-68: Adds LCS and NW Algorithm similarity% in front-end
</commit_message>
<xml_diff>
--- a/plagiarism-detector/src/test/resources/studentData.xlsx
+++ b/plagiarism-detector/src/test/resources/studentData.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{B4C51E10-F811-4730-9402-B0D82D5FAC73}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B581A985-D4B4-4642-B68F-FF02BED6F132}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10700" windowHeight="3440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10704" windowHeight="3444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -53,12 +52,6 @@
     <t>g</t>
   </si>
   <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
     <t>Darshan</t>
   </si>
   <si>
@@ -69,6 +62,18 @@
   </si>
   <si>
     <t>John</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>max@x.com</t>
+  </si>
+  <si>
+    <t>Kat</t>
+  </si>
+  <si>
+    <t>kat@x.com</t>
   </si>
 </sst>
 </file>
@@ -400,17 +405,17 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="37.7265625" customWidth="1"/>
+    <col min="3" max="3" width="37.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -421,18 +426,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>102</v>
       </c>
@@ -443,40 +448,40 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>106</v>
       </c>
@@ -487,7 +492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>107</v>
       </c>
@@ -498,7 +503,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>108</v>
       </c>
@@ -509,7 +514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>109</v>
       </c>
@@ -520,26 +525,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -547,6 +552,8 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{581B82DA-27AD-49F8-8A44-CE28843FEAE7}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{EFFF7434-BFAF-4AF7-A67E-C9D673399FC5}"/>
     <hyperlink ref="C4:C12" r:id="rId3" display="s.sh@husky.neu.edu" xr:uid="{62E31CEB-996A-4364-A522-6D95F8C3495A}"/>
+    <hyperlink ref="C11" r:id="rId4" xr:uid="{B04AB849-43F4-4F97-A1CE-E7A5AFB10CC6}"/>
+    <hyperlink ref="C12" r:id="rId5" xr:uid="{54562882-42BA-4807-BBD4-E012DBC5B6BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added machine learning using moss and minor refactoring
</commit_message>
<xml_diff>
--- a/plagiarism-detector/src/test/resources/studentData.xlsx
+++ b/plagiarism-detector/src/test/resources/studentData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F20F9F6-B9E4-4632-972A-ECB45AD163F7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1871A31B-1388-42CF-840F-09A215DED233}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10704" windowHeight="3444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10700" windowHeight="3440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>kat@x.com</t>
   </si>
   <si>
-    <t>pasne.d@husky.neu.edu</t>
-  </si>
-  <si>
     <t>sood.s@husky.neu.edu</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>hawking.g@husky.neu.edu</t>
+  </si>
+  <si>
+    <t>panse.d@husky.neu.edu</t>
   </si>
 </sst>
 </file>
@@ -426,17 +426,17 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" customWidth="1"/>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="3" max="3" width="37.77734375" customWidth="1"/>
+    <col min="3" max="3" width="37.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>101</v>
       </c>
@@ -455,10 +455,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>102</v>
       </c>
@@ -466,10 +466,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>103</v>
       </c>
@@ -477,10 +477,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>104</v>
       </c>
@@ -488,10 +488,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>105</v>
       </c>
@@ -499,54 +499,54 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>110</v>
       </c>
@@ -557,7 +557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>111</v>
       </c>

</xml_diff>